<commit_message>
Updated to the recent Bioc 3.23.
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremychacon/Dropbox/RIS/projects/multieditR/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanek/Rpacks/multieditR_Package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53182C2A-7722-F54A-8E87-A70EA39EB515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C77AED-4170-FD44-98EC-5A38FDFF7F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2220" windowWidth="17220" windowHeight="11780" xr2:uid="{5DC8A414-0A15-2B42-9817-CC62D9680170}"/>
+    <workbookView xWindow="2760" yWindow="2220" windowWidth="42040" windowHeight="27080" xr2:uid="{5DC8A414-0A15-2B42-9817-CC62D9680170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,12 +78,6 @@
     <t>CCATCTCTAACAAAAATACG</t>
   </si>
   <si>
-    <t>4 Round 1_B01.ab1</t>
-  </si>
-  <si>
-    <t>4 Round 1_B01_ctrl.fasta</t>
-  </si>
-  <si>
     <t>Test9</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>phred_cutoff</t>
+  </si>
+  <si>
+    <t>4_Round_1_B01.ab1</t>
+  </si>
+  <si>
+    <t>4_Round_1_B01_ctrl.fasta</t>
   </si>
 </sst>
 </file>
@@ -187,9 +187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -333,7 +333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,7 +485,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE5656A-6A32-8B49-8F45-780B1A222171}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -500,31 +502,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -761,25 +763,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10">
         <v>0.01</v>
@@ -790,16 +792,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>

</xml_diff>